<commit_message>
mise à jour accès
</commit_message>
<xml_diff>
--- a/acces-gcp.xlsx
+++ b/acces-gcp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihab/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utopios/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41E5DF0-835C-4943-91E9-B1105993BC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A779841-3F92-8145-9DC9-2DBD3756FC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{749FE160-EDD4-264A-A4FC-E490144C1BDE}"/>
+    <workbookView xWindow="55160" yWindow="3420" windowWidth="28040" windowHeight="16100" xr2:uid="{749FE160-EDD4-264A-A4FC-E490144C1BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>e1u1@utopios.solutions</t>
   </si>
@@ -70,9 +69,6 @@
     <t>PK3gD&gt;GE</t>
   </si>
   <si>
-    <t>VCj*2Eqj</t>
-  </si>
-  <si>
     <t>e1u2@utopios.solutions</t>
   </si>
   <si>
@@ -88,7 +84,28 @@
     <t>e3u2@utopios.solutions</t>
   </si>
   <si>
-    <t>e3u3@utopios.solutions</t>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>SODKI</t>
+  </si>
+  <si>
+    <t>Viktoriia</t>
+  </si>
+  <si>
+    <t>Haroun</t>
+  </si>
+  <si>
+    <t>Salma</t>
+  </si>
+  <si>
+    <t>Said</t>
+  </si>
+  <si>
+    <t>Imed</t>
+  </si>
+  <si>
+    <t>Yacine</t>
   </si>
 </sst>
 </file>
@@ -458,88 +475,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA646A3C-D623-D747-B61F-386F9EA8165B}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="1" max="1" width="42.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -549,7 +587,6 @@
     <hyperlink ref="A6" r:id="rId4" xr:uid="{57E7BED0-E1A2-324E-A661-5565F907175B}"/>
     <hyperlink ref="A7" r:id="rId5" xr:uid="{587BCF9F-A0FF-ED4D-A575-1C7EF7910CBB}"/>
     <hyperlink ref="A8" r:id="rId6" xr:uid="{F76BF342-7C79-3745-B3BC-AEC630FEB5E6}"/>
-    <hyperlink ref="A9" r:id="rId7" xr:uid="{A4E48228-1296-9747-8F85-2A9D9229BE2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>